<commit_message>
added excel config 2
</commit_message>
<xml_diff>
--- a/src/test/resources/NewEventTest.xlsx
+++ b/src/test/resources/NewEventTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Title</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Minutes</t>
   </si>
   <si>
-    <t>Shanawaz</t>
-  </si>
-  <si>
     <t>Critical</t>
   </si>
   <si>
@@ -93,25 +90,55 @@
     <t>1 Hour</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
     <t>Shanawaz Mansuri (shanawazmansuri)</t>
   </si>
   <si>
     <t>Via Text Message</t>
   </si>
   <si>
-    <t>FromDate</t>
-  </si>
-  <si>
-    <t>ToDate</t>
-  </si>
-  <si>
-    <t>10/5/2018  10:32:00 AM</t>
-  </si>
-  <si>
-    <t>11/5/2018  10:32:00 AM</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>##</t>
+  </si>
+  <si>
+    <t>$$</t>
+  </si>
+  <si>
+    <t>!!</t>
+  </si>
+  <si>
+    <t>Test11$</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>From Date</t>
+  </si>
+  <si>
+    <t>To Date</t>
+  </si>
+  <si>
+    <t>02-Apr-2018  10:20</t>
+  </si>
+  <si>
+    <t>05-Apr-2018  10:21</t>
   </si>
 </sst>
 </file>
@@ -119,7 +146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy\ h:mm"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -152,8 +179,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,13 +478,14 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="5" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="36.28515625" bestFit="1" customWidth="1"/>
@@ -468,16 +496,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -532,71 +560,71 @@
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="V2" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>